<commit_message>
Align payroll excel file with hrapp
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/payslip.xlsx
+++ b/src/main/resources/excel/payslip.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\hrapp\src\main\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360F2206-D679-4F0A-99DE-A1234C43BEE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="255" windowWidth="19035" windowHeight="9480"/>
+    <workbookView xWindow="0" yWindow="252" windowWidth="19032" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
-  <si>
-    <t>TOTAL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="1">
   <si>
     <t>EMPLOYEE NAME</t>
   </si>
@@ -26,11 +31,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -163,28 +168,27 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -197,9 +201,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -208,6 +211,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -254,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,9 +297,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,6 +349,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,64 +542,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.95" customHeight="1">
+    <row r="1" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="6"/>
       <c r="G1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A2" s="31">
+    <row r="2" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
         <v>42005</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="31">
+      <c r="D2" s="29">
         <v>42005</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="31">
+      <c r="G2" s="29">
         <v>42005</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="12.95" customHeight="1">
+    <row r="3" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="29"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="7"/>
@@ -560,10 +605,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="12.95" customHeight="1">
+    <row r="4" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="29"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="1"/>
       <c r="E4" s="12"/>
       <c r="F4" s="7"/>
@@ -571,153 +616,138 @@
       <c r="H4" s="12"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="1"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="1"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="1"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="20"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="1"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="1"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="1"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="1"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="1"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="1"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A11" s="19"/>
+    <row r="11" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1"/>
       <c r="F11" s="7"/>
       <c r="G11" s="14"/>
       <c r="H11" s="1"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A12" s="19"/>
+    <row r="12" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="7"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.95" customHeight="1">
+    <row r="13" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.95" customHeight="1">
+    <row r="14" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="7"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.95" customHeight="1">
+    <row r="15" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="32">
-        <f>SUM(C4:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="32">
-        <f>SUM(F4:F15)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="16">
-        <f>SUM(I4:I15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="8"/>
@@ -728,41 +758,41 @@
       <c r="H17" s="2"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="12.95" customHeight="1">
+    <row r="18" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A19" s="31">
+    <row r="19" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
         <v>42005</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="31">
+      <c r="D19" s="29">
         <v>42005</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <v>42005</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="12.95" customHeight="1">
+    <row r="20" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7"/>
@@ -773,7 +803,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="12.95" customHeight="1">
+    <row r="21" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="7"/>
@@ -784,105 +814,105 @@
       <c r="H21" s="12"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A22" s="27"/>
+    <row r="22" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
       <c r="B22" s="1"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="22"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="1"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="1"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
       <c r="B24" s="1"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="1"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="25"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
       <c r="B25" s="1"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="1"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="1"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A26" s="19"/>
+    <row r="26" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
       <c r="B26" s="1"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="1"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="21"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="1"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A27" s="19"/>
+    <row r="27" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
       <c r="B27" s="1"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="21"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="1"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A28" s="19"/>
+    <row r="28" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
       <c r="B28" s="1"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="1"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="1"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" ht="12.95" customHeight="1">
+    <row r="29" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="1"/>
       <c r="F29" s="7"/>
       <c r="G29" s="13"/>
       <c r="H29" s="1"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" ht="12.95" customHeight="1">
+    <row r="30" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="1"/>
       <c r="F30" s="7"/>
       <c r="G30" s="14"/>
       <c r="H30" s="1"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="12.95" customHeight="1">
+    <row r="31" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="1"/>
       <c r="C31" s="7"/>
@@ -893,44 +923,29 @@
       <c r="H31" s="1"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="12.95" customHeight="1">
+    <row r="32" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="30"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="30"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="30"/>
-    </row>
-    <row r="33" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="16">
-        <f>SUM(C21:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="16">
-        <f>SUM(F21:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="4"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="16">
-        <f>SUM(I21:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="2"/>
       <c r="C34" s="8"/>
@@ -941,41 +956,41 @@
       <c r="H34" s="2"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="1:9" ht="12.95" customHeight="1">
+    <row r="35" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="7"/>
       <c r="D35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A36" s="31">
+    <row r="36" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
         <v>42005</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="31">
+      <c r="D36" s="29">
         <v>42005</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="31">
+      <c r="G36" s="29">
         <v>42005</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="12.95" customHeight="1">
+    <row r="37" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
@@ -983,7 +998,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="12.95" customHeight="1">
+    <row r="38" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="7"/>
@@ -994,145 +1009,130 @@
       <c r="H38" s="12"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A39" s="27"/>
+    <row r="39" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
       <c r="B39" s="1"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="28"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="1"/>
       <c r="F39" s="7"/>
       <c r="G39" s="1"/>
       <c r="H39" s="12"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
       <c r="B40" s="1"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="21"/>
-      <c r="G40" s="24"/>
+      <c r="D40" s="20"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A41" s="19"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
       <c r="B41" s="1"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="21"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="1"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="42" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A42" s="19"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
       <c r="B42" s="1"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="21"/>
-      <c r="G42" s="25"/>
+      <c r="D42" s="20"/>
+      <c r="G42" s="24"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="17"/>
-    </row>
-    <row r="43" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A43" s="19"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
       <c r="B43" s="1"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="21"/>
-      <c r="G43" s="24"/>
+      <c r="D43" s="20"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="17"/>
-    </row>
-    <row r="44" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="1"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="21"/>
-      <c r="G44" s="24"/>
+      <c r="D44" s="20"/>
+      <c r="G44" s="23"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="17"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="1"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="21"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="1"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="24"/>
+      <c r="G45" s="23"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" ht="12.95" customHeight="1">
+    <row r="46" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="1"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="21"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="1"/>
       <c r="F46" s="7"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="17"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="21"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="1"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="24"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="17"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="1"/>
       <c r="C48" s="7"/>
-      <c r="D48" s="21"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="1"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="24"/>
+      <c r="G48" s="23"/>
       <c r="H48" s="1"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" ht="12.95" customHeight="1">
+    <row r="49" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="30"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="14"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="20"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="30"/>
-    </row>
-    <row r="50" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="16">
-        <f>SUM(C38:C49)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="4"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="16">
-        <f>SUM(F38:F49)</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F50" s="30"/>
+      <c r="G50" s="4"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="16">
-        <f>SUM(I38:I49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="8"/>
@@ -1143,7 +1143,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="1:9" ht="12.95" customHeight="1">
+    <row r="52" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="1"/>
@@ -1157,64 +1157,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.95" customHeight="1">
+    <row r="1" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="6"/>
       <c r="G1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A2" s="31">
+    <row r="2" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
         <v>42005</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="31">
+      <c r="D2" s="29">
         <v>42005</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="31">
+      <c r="G2" s="29">
         <v>42005</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="12.95" customHeight="1">
+    <row r="3" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="29"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="7"/>
@@ -1222,10 +1220,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="12.95" customHeight="1">
+    <row r="4" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="29"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="1"/>
       <c r="E4" s="12"/>
       <c r="F4" s="7"/>
@@ -1233,153 +1231,138 @@
       <c r="H4" s="12"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="1"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="1"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="1"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="20"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="1"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="1"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="1"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="1"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="1"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="1"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A11" s="19"/>
+    <row r="11" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1"/>
       <c r="F11" s="7"/>
       <c r="G11" s="14"/>
       <c r="H11" s="1"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A12" s="19"/>
+    <row r="12" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="7"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.95" customHeight="1">
+    <row r="13" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="7"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.95" customHeight="1">
+    <row r="14" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="7"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.95" customHeight="1">
+    <row r="15" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="32">
-        <f>SUM(C4:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="32">
-        <f>SUM(F4:F15)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="16">
-        <f>SUM(I4:I15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="8"/>
@@ -1390,41 +1373,41 @@
       <c r="H17" s="2"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="12.95" customHeight="1">
+    <row r="18" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A19" s="31">
+    <row r="19" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
         <v>42005</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="31">
+      <c r="D19" s="29">
         <v>42005</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <v>42005</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="12.95" customHeight="1">
+    <row r="20" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7"/>
@@ -1435,7 +1418,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="12.95" customHeight="1">
+    <row r="21" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="7"/>
@@ -1446,105 +1429,105 @@
       <c r="H21" s="12"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A22" s="27"/>
+    <row r="22" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
       <c r="B22" s="1"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="22"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="1"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="1"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
       <c r="B24" s="1"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="1"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="25"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
       <c r="B25" s="1"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="1"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="1"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A26" s="19"/>
+    <row r="26" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
       <c r="B26" s="1"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="1"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="21"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="1"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A27" s="19"/>
+    <row r="27" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
       <c r="B27" s="1"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="21"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="1"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A28" s="19"/>
+    <row r="28" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
       <c r="B28" s="1"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="1"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="1"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" ht="12.95" customHeight="1">
+    <row r="29" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="1"/>
       <c r="F29" s="7"/>
       <c r="G29" s="13"/>
       <c r="H29" s="1"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" ht="12.95" customHeight="1">
+    <row r="30" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="1"/>
       <c r="F30" s="7"/>
       <c r="G30" s="14"/>
       <c r="H30" s="1"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="12.95" customHeight="1">
+    <row r="31" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="1"/>
       <c r="C31" s="7"/>
@@ -1555,44 +1538,29 @@
       <c r="H31" s="1"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="12.95" customHeight="1">
+    <row r="32" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="30"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="30"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="30"/>
-    </row>
-    <row r="33" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="16">
-        <f>SUM(C21:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="16">
-        <f>SUM(F21:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="4"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="16">
-        <f>SUM(I21:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="2"/>
       <c r="C34" s="8"/>
@@ -1603,41 +1571,41 @@
       <c r="H34" s="2"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="1:9" ht="12.95" customHeight="1">
+    <row r="35" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="7"/>
       <c r="D35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="7"/>
       <c r="G35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A36" s="31">
+    <row r="36" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
         <v>42005</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="31">
+      <c r="D36" s="29">
         <v>42005</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="31">
+      <c r="G36" s="29">
         <v>42005</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="12.95" customHeight="1">
+    <row r="37" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
@@ -1645,7 +1613,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="12.95" customHeight="1">
+    <row r="38" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="7"/>
@@ -1656,145 +1624,130 @@
       <c r="H38" s="12"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A39" s="27"/>
+    <row r="39" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
       <c r="B39" s="1"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="28"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="1"/>
       <c r="F39" s="7"/>
       <c r="G39" s="1"/>
       <c r="H39" s="12"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
       <c r="B40" s="1"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="21"/>
-      <c r="G40" s="24"/>
+      <c r="D40" s="20"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A41" s="19"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
       <c r="B41" s="1"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="21"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="1"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="42" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A42" s="19"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
       <c r="B42" s="1"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="21"/>
-      <c r="G42" s="25"/>
+      <c r="D42" s="20"/>
+      <c r="G42" s="24"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="17"/>
-    </row>
-    <row r="43" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A43" s="19"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
       <c r="B43" s="1"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="21"/>
-      <c r="G43" s="24"/>
+      <c r="D43" s="20"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="17"/>
-    </row>
-    <row r="44" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="1"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="21"/>
-      <c r="G44" s="24"/>
+      <c r="D44" s="20"/>
+      <c r="G44" s="23"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="17"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="1"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="21"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="1"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="24"/>
+      <c r="G45" s="23"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" ht="12.95" customHeight="1">
+    <row r="46" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="1"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="21"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="1"/>
       <c r="F46" s="7"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="17"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="21"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="1"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="24"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="17"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="1"/>
       <c r="C48" s="7"/>
-      <c r="D48" s="21"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="1"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="24"/>
+      <c r="G48" s="23"/>
       <c r="H48" s="1"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" ht="12.95" customHeight="1">
+    <row r="49" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="30"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="14"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="20"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="30"/>
-    </row>
-    <row r="50" spans="1:9" ht="12.95" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="16">
-        <f>SUM(C38:C49)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="4"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="16">
-        <f>SUM(F38:F49)</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="F50" s="30"/>
+      <c r="G50" s="4"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="16">
-        <f>SUM(I38:I49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="12.95" customHeight="1">
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="8"/>
@@ -1805,7 +1758,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="1:9" ht="12.95" customHeight="1">
+    <row r="52" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="1"/>
@@ -1815,4 +1768,1226 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C48004-B1E5-405D-9907-7460CBC9EB32}">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="25"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="7"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="20"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="20"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="20"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="20"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="23"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4F4F1B-F9B3-415E-8AA5-22F4B1979578}">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="25"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="29">
+        <v>42005</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="7"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="20"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="20"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="20"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="20"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="23"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>